<commit_message>
change Sri Lank's score for VGGT 16-3c to a score of B (it is currently a C)
</commit_message>
<xml_diff>
--- a/Simple_XLS_Importer/data/NKT-VGGT16/2017-NKT-VGGT-16.3.xlsx
+++ b/Simple_XLS_Importer/data/NKT-VGGT16/2017-NKT-VGGT-16.3.xlsx
@@ -6409,8 +6409,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J960"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A50" sqref="A1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A141" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D142" sqref="D142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -8922,8 +8922,8 @@
       <c r="C142" s="22">
         <v>2017</v>
       </c>
-      <c r="D142" s="30" t="s">
-        <v>40</v>
+      <c r="D142" s="31" t="s">
+        <v>39</v>
       </c>
       <c r="E142" s="41" t="s">
         <v>129</v>

</xml_diff>

<commit_message>
changed value for VGGT16-3e Taiwan
</commit_message>
<xml_diff>
--- a/Simple_XLS_Importer/data/NKT-VGGT16/2017-NKT-VGGT-16.3.xlsx
+++ b/Simple_XLS_Importer/data/NKT-VGGT16/2017-NKT-VGGT-16.3.xlsx
@@ -6413,8 +6413,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J960"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A277" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E294" activeCellId="1" sqref="E294 E294"/>
+    <sheetView tabSelected="1" topLeftCell="A236" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D244" sqref="D244"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -10762,8 +10762,8 @@
       <c r="C244" s="22">
         <v>2017</v>
       </c>
-      <c r="D244" s="29" t="s">
-        <v>38</v>
+      <c r="D244" s="31" t="s">
+        <v>39</v>
       </c>
       <c r="E244" s="42" t="s">
         <v>419</v>
@@ -16556,7 +16556,7 @@
       <c r="E960" s="39"/>
     </row>
   </sheetData>
-  <dataValidations disablePrompts="1" count="2">
+  <dataValidations count="2">
     <dataValidation type="list" sqref="C2:C22 C24:C93 C95:C193 C195:C243 C245:C393 C395:C443 C445:C451">
       <formula1>#REF!</formula1>
     </dataValidation>

</xml_diff>

<commit_message>
change Peru's score for 16.3e (right to negotiate) from a B to a C. NKT-VGGT16
</commit_message>
<xml_diff>
--- a/Simple_XLS_Importer/data/NKT-VGGT16/2017-NKT-VGGT-16.3.xlsx
+++ b/Simple_XLS_Importer/data/NKT-VGGT16/2017-NKT-VGGT-16.3.xlsx
@@ -6413,8 +6413,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J960"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A236" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D244" sqref="D244"/>
+    <sheetView tabSelected="1" topLeftCell="A230" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D236" sqref="D236"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -10618,8 +10618,8 @@
       <c r="C236" s="22">
         <v>2017</v>
       </c>
-      <c r="D236" s="31" t="s">
-        <v>39</v>
+      <c r="D236" s="30" t="s">
+        <v>40</v>
       </c>
       <c r="E236" s="38" t="s">
         <v>282</v>

</xml_diff>